<commit_message>
Revise Lesson 12 and the associated data files.
</commit_message>
<xml_diff>
--- a/Data/DirectFlightCosts.xlsx
+++ b/Data/DirectFlightCosts.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\BYUI_M221_Book_R\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0445817F-A57E-4BCD-8C38-8D96D2AEAF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="8400" windowHeight="2400"/>
+    <workbookView xWindow="-25725" yWindow="-1890" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="107">
   <si>
     <t>Origin</t>
   </si>
@@ -334,12 +340,15 @@
   </si>
   <si>
     <t>Zürich Airport</t>
+  </si>
+  <si>
+    <t>Renamed: flight_costs.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,6 +389,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -428,7 +440,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,9 +473,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,6 +525,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -671,14 +717,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -712,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -729,7 +777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -746,7 +794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -760,7 +808,7 @@
         <v>270.19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -777,7 +825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -794,7 +842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -811,7 +859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -828,7 +876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -845,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -859,7 +907,7 @@
         <v>95.39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -876,7 +924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -887,7 +935,7 @@
         <v>303.69</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -904,7 +952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -918,7 +966,7 @@
         <v>194.49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -931,8 +979,11 @@
       <c r="D16">
         <v>129.59</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -946,7 +997,7 @@
         <v>139.59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -960,7 +1011,7 @@
         <v>318.08999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -974,7 +1025,7 @@
         <v>1242.0899999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -988,7 +1039,7 @@
         <v>113.99</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1002,7 +1053,7 @@
         <v>146.59</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1016,7 +1067,7 @@
         <v>378.09</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1030,7 +1081,7 @@
         <v>306.39</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1044,7 +1095,7 @@
         <v>226.99</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1058,7 +1109,7 @@
         <v>114.59</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +1123,7 @@
         <v>270.19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1086,7 +1137,7 @@
         <v>793.79</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1100,7 +1151,7 @@
         <v>87.49</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1114,7 +1165,7 @@
         <v>104.19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1128,7 +1179,7 @@
         <v>86.39</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1193,7 @@
         <v>265.19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1156,7 +1207,7 @@
         <v>107.59</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1221,7 @@
         <v>194.49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1184,7 +1235,7 @@
         <v>230.09</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1198,7 +1249,7 @@
         <v>96.19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1263,7 @@
         <v>138.69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1223,7 +1274,7 @@
         <v>263.08999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1237,7 +1288,7 @@
         <v>192.59</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1251,7 +1302,7 @@
         <v>106.59</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1265,7 +1316,7 @@
         <v>106.59</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1279,7 +1330,7 @@
         <v>109.59</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1344,7 @@
         <v>183.09</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1358,7 @@
         <v>123.69</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1321,7 +1372,7 @@
         <v>143.59</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1335,7 +1386,7 @@
         <v>199.69</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1349,7 +1400,7 @@
         <v>184.59</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1363,7 +1414,7 @@
         <v>326.39</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1377,7 +1428,7 @@
         <v>118.59</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1391,7 +1442,7 @@
         <v>263.08999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1405,7 +1456,7 @@
         <v>210.09</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1419,7 +1470,7 @@
         <v>170.59</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1484,7 @@
         <v>164.59</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1447,7 +1498,7 @@
         <v>150.59</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1455,7 +1506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1469,7 +1520,7 @@
         <v>183.09</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1534,7 @@
         <v>129.59</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1497,7 +1548,7 @@
         <v>194.49</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1511,7 +1562,7 @@
         <v>164.59</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +1576,7 @@
         <v>230.69</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1539,7 +1590,7 @@
         <v>72.290000000000006</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1553,7 +1604,7 @@
         <v>188.69</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1567,7 +1618,7 @@
         <v>148.88999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1581,7 +1632,7 @@
         <v>298.49</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -1595,7 +1646,7 @@
         <v>106.59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1609,7 +1660,7 @@
         <v>136.59</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1623,7 +1674,7 @@
         <v>250.29</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1637,7 +1688,7 @@
         <v>1176.99</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1651,7 +1702,7 @@
         <v>131.59</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1716,7 @@
         <v>281.08999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1679,7 +1730,7 @@
         <v>286.99</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1744,7 @@
         <v>114.59</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1758,7 @@
         <v>104.59</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1772,7 @@
         <v>721.34</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -1735,7 +1786,7 @@
         <v>188.59</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -1749,7 +1800,7 @@
         <v>210.89</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -1763,7 +1814,7 @@
         <v>175.59</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1828,7 @@
         <v>296.19</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1791,7 +1842,7 @@
         <v>330.49</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1805,7 +1856,7 @@
         <v>782.09</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1819,7 +1870,7 @@
         <v>121.59</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -1833,7 +1884,7 @@
         <v>120.59</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -1847,7 +1898,7 @@
         <v>124.19</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -1861,7 +1912,7 @@
         <v>240.09</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -1875,7 +1926,7 @@
         <v>180.59</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -1889,7 +1940,7 @@
         <v>194.89</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -1903,7 +1954,7 @@
         <v>354.69</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -1917,7 +1968,7 @@
         <v>194.49</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -1931,7 +1982,7 @@
         <v>283.58999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -1945,7 +1996,7 @@
         <v>128.59</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +2010,7 @@
         <v>341.89</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -1979,24 +2030,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>